<commit_message>
2025.01.18_2 After major breakdown and screen burst
</commit_message>
<xml_diff>
--- a/Analysis/bia_baseline.xlsx
+++ b/Analysis/bia_baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavosplmoura/Library/Mobile Documents/com~apple~CloudDocs/Medicina/Biblioteca/Research/Data Science/Data Science/PROJECTS/DVEP/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E5B04653-D3DC-FE47-92D0-EE0EF9B6B85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC20929-351B-CB4A-8BF9-9C418B50B490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="620" windowWidth="46520" windowHeight="25040" activeTab="3" xr2:uid="{FD799774-BD8C-8548-A615-459C767A3F24}"/>
+    <workbookView xWindow="16840" yWindow="6080" windowWidth="24280" windowHeight="19060" activeTab="2" xr2:uid="{FD799774-BD8C-8548-A615-459C767A3F24}"/>
   </bookViews>
   <sheets>
     <sheet name="bia_baseline" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="343">
   <si>
     <t>record_id</t>
   </si>
@@ -1000,6 +1000,75 @@
   </si>
   <si>
     <t>Comparação da análise de impedância bioelétrica corporal basal dos participantes de pesquisa do sexo feminino, conforme o grupo de alocação.</t>
+  </si>
+  <si>
+    <t>Altura (m)</t>
+  </si>
+  <si>
+    <t>Peso (kg)</t>
+  </si>
+  <si>
+    <t>Índice de Massa Corporal (kg/m²)</t>
+  </si>
+  <si>
+    <t>Circunferência Abdominal (m)</t>
+  </si>
+  <si>
+    <t>Nível de Atividade Física (PAL)</t>
+  </si>
+  <si>
+    <t>Ângulo de Fase (°)</t>
+  </si>
+  <si>
+    <t>Resistência (Ω)</t>
+  </si>
+  <si>
+    <t>Reatância (Ω)</t>
+  </si>
+  <si>
+    <t>Massa gorda Absoluta (kg)</t>
+  </si>
+  <si>
+    <t>Índice de Massa gorda (kg/m²)</t>
+  </si>
+  <si>
+    <t>Massa gorda Relativa (%)</t>
+  </si>
+  <si>
+    <t>Tecido Adiposo Visceral (kg)</t>
+  </si>
+  <si>
+    <t>Massa Livre de Gordura Absoluta (kg)</t>
+  </si>
+  <si>
+    <t>Índice de Massa Livre de Gordura (kg/m²)</t>
+  </si>
+  <si>
+    <t>Massa Livre de Gordura Relativa (%)</t>
+  </si>
+  <si>
+    <t>MME Corporal Total (kg)</t>
+  </si>
+  <si>
+    <t>MME do Tronco (kg)</t>
+  </si>
+  <si>
+    <t>MME do Braço Direito (kg)</t>
+  </si>
+  <si>
+    <t>MME do Braço Esquerdo (kg)</t>
+  </si>
+  <si>
+    <t>MME da Perna Direita (kg)</t>
+  </si>
+  <si>
+    <t>MME da Perna Esquerda (kg)</t>
+  </si>
+  <si>
+    <t>Água Corporal Total (L)</t>
+  </si>
+  <si>
+    <t>Água Extracelular (L)</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1076,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1145,16 +1214,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Century Schoolbook"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Light"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1350,7 +1417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1542,6 +1609,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1587,35 +1665,43 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1661,7 +1747,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1678,22 +1764,7 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1723,7 +1794,7 @@
     <tableColumn id="6" xr3:uid="{FFB3A7D9-22B4-0246-9D3B-1D8C8790EDB6}" name="Valor p">
       <calculatedColumnFormula>IF(G2&lt;0.05,CONCATENATE(ROUND(G2,3),"*"),ROUND(G2,3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5683314D-CA2B-D145-B409-4EB68872F93E}" name="Valor p2" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{5683314D-CA2B-D145-B409-4EB68872F93E}" name="Valor p2" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1988,9 +2059,9 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2079,7 +2150,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2168,7 +2239,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2257,7 +2328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2346,7 +2417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2435,7 +2506,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2524,7 +2595,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2613,7 +2684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2702,7 +2773,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2791,7 +2862,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2880,7 +2951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2969,7 +3040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3058,7 +3129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3147,7 +3218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3236,7 +3307,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3325,7 +3396,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3414,7 +3485,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3503,7 +3574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3592,7 +3663,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3681,7 +3752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3770,7 +3841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3859,7 +3930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3948,7 +4019,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4037,7 +4108,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4126,7 +4197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4215,7 +4286,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4304,7 +4375,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4393,7 +4464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4482,7 +4553,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4571,7 +4642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4660,7 +4731,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4749,7 +4820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4838,7 +4909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4927,7 +4998,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5016,7 +5087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5105,7 +5176,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5194,7 +5265,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5283,7 +5354,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5372,7 +5443,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5461,7 +5532,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5550,7 +5621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5639,7 +5710,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5728,7 +5799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5817,7 +5888,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5906,7 +5977,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5995,7 +6066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6084,7 +6155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6173,7 +6244,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6262,7 +6333,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6351,7 +6422,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6440,7 +6511,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6529,7 +6600,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6618,7 +6689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6707,7 +6778,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6796,7 +6867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6885,7 +6956,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6974,7 +7045,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>56</v>
       </c>
@@ -7063,7 +7134,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>57</v>
       </c>
@@ -7152,7 +7223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>58</v>
       </c>
@@ -7241,7 +7312,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>59</v>
       </c>
@@ -7330,7 +7401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>60</v>
       </c>
@@ -7419,7 +7490,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>61</v>
       </c>
@@ -7508,7 +7579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>62</v>
       </c>
@@ -7597,7 +7668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>63</v>
       </c>
@@ -7686,7 +7757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>64</v>
       </c>
@@ -7775,7 +7846,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>65</v>
       </c>
@@ -7864,7 +7935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>66</v>
       </c>
@@ -7953,7 +8024,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>67</v>
       </c>
@@ -8042,7 +8113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>68</v>
       </c>
@@ -8131,7 +8202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>69</v>
       </c>
@@ -8220,7 +8291,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>70</v>
       </c>
@@ -8309,7 +8380,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>71</v>
       </c>
@@ -8398,7 +8469,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8487,7 +8558,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8576,7 +8647,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>74</v>
       </c>
@@ -8665,7 +8736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:29" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8761,20 +8832,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF158CB-E912-B44A-B12F-04C4E260788C}">
-  <dimension ref="C1:H28"/>
+  <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView zoomScale="139" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C25"/>
+      <selection activeCell="G3" sqref="G3:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:11" ht="28" x14ac:dyDescent="0.15">
       <c r="C1" t="s">
         <v>202</v>
       </c>
@@ -8794,7 +8866,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>205</v>
       </c>
@@ -8805,560 +8877,647 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
+        <v>320</v>
+      </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F3">
-        <v>-4.22</v>
+        <v>-7.65</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(H3 &lt; 0.001,"&lt; 0.001", ROUND(H3,3))</f>
-        <v>&lt; 0.001</v>
+        <f>IF(H3&lt;0.001,"&lt; 0.001*",IF(H3&lt;0.05,CONCATENATE(H3,"*"),ROUND(H3,3)))</f>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H3">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="K3" s="22"/>
+    </row>
+    <row r="4" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B4" s="22" t="s">
+        <v>321</v>
+      </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F4">
-        <v>5.21</v>
+        <v>-3.85</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G28" si="0">IF(H4 &lt; 0.001,"&lt; 0.001", ROUND(H4,3))</f>
-        <v>&lt; 0.001</v>
+        <f t="shared" ref="G4:G25" si="0">IF(H4&lt;0.001,"&lt; 0.001*",IF(H4&lt;0.05,CONCATENATE(H4,"*"),ROUND(H4,3)))</f>
+        <v>0.0018*</v>
       </c>
       <c r="H4">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.15">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K4" s="22"/>
+    </row>
+    <row r="5" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B5" s="22" t="s">
+        <v>322</v>
+      </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="F5">
-        <v>2.2599999999999998</v>
+        <v>1.36</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="H5">
-        <v>4.0099999999999997E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.15">
+        <v>0.17760000000000001</v>
+      </c>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B6" s="22" t="s">
+        <v>323</v>
+      </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>211</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F6">
-        <v>-3.85</v>
-      </c>
-      <c r="G6">
+        <v>-3.08</v>
+      </c>
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>2E-3</v>
+        <v>0.0071*</v>
       </c>
       <c r="H6">
-        <v>1.8E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.15">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="22" t="s">
+        <v>324</v>
+      </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F7">
-        <v>-7.65</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.15">
-      <c r="C8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F8">
-        <v>-3.08</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="H8">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.15">
-      <c r="C9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E9" t="s">
-        <v>183</v>
-      </c>
-      <c r="F9">
         <v>-0.48</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>0.64400000000000002</v>
       </c>
+      <c r="H7">
+        <v>0.64359999999999995</v>
+      </c>
+      <c r="K7" s="22"/>
+    </row>
+    <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8">
+        <v>-4.22</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt; 0.001*</v>
+      </c>
+      <c r="H8">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K8" s="21"/>
+    </row>
+    <row r="9" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B9" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9">
+        <v>5.21</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt; 0.001*</v>
+      </c>
       <c r="H9">
-        <v>0.64359999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.15">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K9" s="22"/>
+    </row>
+    <row r="10" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B10" s="22" t="s">
+        <v>327</v>
+      </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F10">
-        <v>1.36</v>
-      </c>
-      <c r="G10" s="3">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>0.17799999999999999</v>
+        <v>0.0401*</v>
       </c>
       <c r="H10">
-        <v>0.17760000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.15">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B11" s="22" t="s">
+        <v>328</v>
+      </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E11" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F11">
-        <v>-4.71</v>
+        <v>3.93</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H11">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.15">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="K11" s="22"/>
+    </row>
+    <row r="12" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B12" s="22" t="s">
+        <v>329</v>
+      </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F12">
-        <v>-13.53</v>
+        <v>5.05</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B13" s="22" t="s">
+        <v>330</v>
+      </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F13">
-        <v>2.84</v>
-      </c>
-      <c r="G13">
+        <v>7.1</v>
+      </c>
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H13">
-        <v>9.7000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B14" s="22" t="s">
+        <v>331</v>
+      </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="E14" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="F14">
-        <v>3.93</v>
+        <v>-5.95</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H14">
-        <v>6.9999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.15">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B15" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F15">
-        <v>5.05</v>
+        <v>-7.31</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K15" s="22"/>
+    </row>
+    <row r="16" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B16" s="22" t="s">
+        <v>333</v>
+      </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F16">
-        <v>7.1</v>
+        <v>-5.12</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.15">
+        <v>1E-4</v>
+      </c>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B17" s="22" t="s">
+        <v>334</v>
+      </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F17">
-        <v>-7.31</v>
+        <v>-7.1</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B18" s="22" t="s">
+        <v>335</v>
+      </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F18">
-        <v>-5.12</v>
+        <v>-8.4</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H18">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B19" s="22" t="s">
+        <v>336</v>
+      </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="D19" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F19">
-        <v>-7.1</v>
+        <v>-7.3</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B20" s="22" t="s">
+        <v>337</v>
+      </c>
       <c r="C20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F20">
-        <v>-8.4</v>
+        <v>-7.54</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K20" s="22"/>
+    </row>
+    <row r="21" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B21" s="22" t="s">
+        <v>338</v>
+      </c>
       <c r="C21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F21">
-        <v>-7.3</v>
+        <v>-7.56</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K21" s="22"/>
+    </row>
+    <row r="22" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B22" s="22" t="s">
+        <v>339</v>
+      </c>
       <c r="C22" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F22">
-        <v>-7.54</v>
+        <v>-8.33</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K22" s="22"/>
+    </row>
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="22" t="s">
+        <v>340</v>
+      </c>
       <c r="C23" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D23" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E23" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F23">
-        <v>-7.56</v>
+        <v>-8.24</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="K23" s="23"/>
+    </row>
+    <row r="24" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B24" s="22" t="s">
+        <v>341</v>
+      </c>
       <c r="C24" t="s">
-        <v>215</v>
+        <v>173</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F24">
-        <v>-8.33</v>
+        <v>-6.89</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
+        <v>&lt; 0.001*</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="23" t="s">
+        <v>342</v>
+      </c>
       <c r="C25" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E25" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F25">
-        <v>-8.24</v>
+        <v>-5.32</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
+        <v>&lt; 0.001*</v>
+      </c>
+      <c r="H25">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="C31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" t="s">
+        <v>185</v>
+      </c>
+      <c r="F31">
+        <v>-4.71</v>
+      </c>
+      <c r="G31" t="str">
+        <f>IF(H31 &lt; 0.001,"&lt; 0.001", ROUND(H31,3))</f>
         <v>&lt; 0.001</v>
       </c>
-      <c r="H25">
+      <c r="H31">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="K31" s="22"/>
+    </row>
+    <row r="32" spans="2:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="C32" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32">
+        <v>-13.53</v>
+      </c>
+      <c r="G32" t="str">
+        <f>IF(H32 &lt; 0.001,"&lt; 0.001", ROUND(H32,3))</f>
+        <v>&lt; 0.001</v>
+      </c>
+      <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.15">
-      <c r="C26" t="s">
-        <v>171</v>
-      </c>
-      <c r="D26" t="s">
-        <v>172</v>
-      </c>
-      <c r="E26" t="s">
-        <v>199</v>
-      </c>
-      <c r="F26">
-        <v>-5.95</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
-      </c>
-      <c r="H26">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.15">
-      <c r="C27" t="s">
-        <v>173</v>
-      </c>
-      <c r="D27" t="s">
-        <v>174</v>
-      </c>
-      <c r="E27" t="s">
-        <v>200</v>
-      </c>
-      <c r="F27">
-        <v>-6.89</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.15">
-      <c r="C28" t="s">
-        <v>175</v>
-      </c>
-      <c r="D28" t="s">
-        <v>176</v>
-      </c>
-      <c r="E28" t="s">
-        <v>201</v>
-      </c>
-      <c r="F28">
-        <v>-5.32</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt; 0.001</v>
-      </c>
-      <c r="H28">
-        <v>2.0000000000000001E-4</v>
-      </c>
+      <c r="K32" s="22"/>
+    </row>
+    <row r="33" spans="3:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="C33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" t="s">
+        <v>153</v>
+      </c>
+      <c r="E33" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33">
+        <v>2.84</v>
+      </c>
+      <c r="G33">
+        <f>IF(H33 &lt; 0.001,"&lt; 0.001", ROUND(H33,3))</f>
+        <v>0.01</v>
+      </c>
+      <c r="H33">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="K33" s="22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="G1:H1 H1:H1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9368,22 +9527,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE52CD2-C5A8-4E4A-B8BB-052C688E70B9}">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="165" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="10.83203125" style="3"/>
     <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>269</v>
       </c>
@@ -9402,7 +9561,7 @@
       <c r="F1" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>270</v>
       </c>
     </row>
@@ -9410,7 +9569,7 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>132</v>
       </c>
       <c r="C2" t="s">
@@ -9423,17 +9582,17 @@
         <v>2.54</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(G2&lt;0.05,CONCATENATE(ROUND(G2,3),"*"),ROUND(G2,3))</f>
+        <f t="shared" ref="F2:F27" si="0">IF(G2&lt;0.05,CONCATENATE(ROUND(G2,3),"*"),ROUND(G2,3))</f>
         <v>0.035*</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>3.49E-2</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.15">
       <c r="A3">
@@ -9452,17 +9611,17 @@
         <v>1.74</v>
       </c>
       <c r="F3">
-        <f>IF(G3&lt;0.05,CONCATENATE(ROUND(G3,3),"*"),ROUND(G3,3))</f>
+        <f t="shared" si="0"/>
         <v>0.122</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.1222</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -9481,23 +9640,23 @@
         <v>2.82</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(G4&lt;0.05,CONCATENATE(ROUND(G4,3),"*"),ROUND(G4,3))</f>
+        <f t="shared" si="0"/>
         <v>0.026*</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>2.58E-2</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>138</v>
       </c>
       <c r="C5" t="s">
@@ -9510,14 +9669,14 @@
         <v>-2.72</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(G5&lt;0.05,CONCATENATE(ROUND(G5,3),"*"),ROUND(G5,3))</f>
+        <f t="shared" si="0"/>
         <v>0.026*</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>2.64E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>6</v>
       </c>
@@ -9534,14 +9693,14 @@
         <v>-1.21</v>
       </c>
       <c r="F6">
-        <f>IF(G6&lt;0.05,CONCATENATE(ROUND(G6,3),"*"),ROUND(G6,3))</f>
+        <f t="shared" si="0"/>
         <v>0.26700000000000002</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0.26690000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>7</v>
       </c>
@@ -9558,14 +9717,14 @@
         <v>-0.38</v>
       </c>
       <c r="F7">
-        <f>IF(G7&lt;0.05,CONCATENATE(ROUND(G7,3),"*"),ROUND(G7,3))</f>
+        <f t="shared" si="0"/>
         <v>0.72599999999999998</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>0.7258</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>8</v>
       </c>
@@ -9582,18 +9741,18 @@
         <v>-0.21</v>
       </c>
       <c r="F8">
-        <f>IF(G8&lt;0.05,CONCATENATE(ROUND(G8,3),"*"),ROUND(G8,3))</f>
+        <f t="shared" si="0"/>
         <v>0.84299999999999997</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.84299999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>146</v>
       </c>
       <c r="C9" t="s">
@@ -9606,14 +9765,14 @@
         <v>-2.85</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(G9&lt;0.05,CONCATENATE(ROUND(G9,3),"*"),ROUND(G9,3))</f>
+        <f t="shared" si="0"/>
         <v>0.026*</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>2.5700000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>10</v>
       </c>
@@ -9630,14 +9789,14 @@
         <v>-0.6</v>
       </c>
       <c r="F10">
-        <f>IF(G10&lt;0.05,CONCATENATE(ROUND(G10,3),"*"),ROUND(G10,3))</f>
+        <f t="shared" si="0"/>
         <v>0.58299999999999996</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0.58260000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>11</v>
       </c>
@@ -9654,14 +9813,14 @@
         <v>-2.33</v>
       </c>
       <c r="F11" t="str">
-        <f>IF(G11&lt;0.05,CONCATENATE(ROUND(G11,3),"*"),ROUND(G11,3))</f>
+        <f t="shared" si="0"/>
         <v>0.048*</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>12</v>
       </c>
@@ -9678,14 +9837,14 @@
         <v>-0.43</v>
       </c>
       <c r="F12">
-        <f>IF(G12&lt;0.05,CONCATENATE(ROUND(G12,3),"*"),ROUND(G12,3))</f>
+        <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>0.68989999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>13</v>
       </c>
@@ -9702,14 +9861,14 @@
         <v>-0.09</v>
       </c>
       <c r="F13">
-        <f>IF(G13&lt;0.05,CONCATENATE(ROUND(G13,3),"*"),ROUND(G13,3))</f>
+        <f t="shared" si="0"/>
         <v>0.93400000000000005</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>0.93440000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>14</v>
       </c>
@@ -9726,14 +9885,14 @@
         <v>0.21</v>
       </c>
       <c r="F14">
-        <f>IF(G14&lt;0.05,CONCATENATE(ROUND(G14,3),"*"),ROUND(G14,3))</f>
+        <f t="shared" si="0"/>
         <v>0.84599999999999997</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>0.84560000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>15</v>
       </c>
@@ -9750,14 +9909,14 @@
         <v>1.01</v>
       </c>
       <c r="F15">
-        <f>IF(G15&lt;0.05,CONCATENATE(ROUND(G15,3),"*"),ROUND(G15,3))</f>
+        <f t="shared" si="0"/>
         <v>0.36199999999999999</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>16</v>
       </c>
@@ -9774,14 +9933,14 @@
         <v>-2.89</v>
       </c>
       <c r="F16" t="str">
-        <f>IF(G16&lt;0.05,CONCATENATE(ROUND(G16,3),"*"),ROUND(G16,3))</f>
+        <f t="shared" si="0"/>
         <v>0.021*</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>17</v>
       </c>
@@ -9798,14 +9957,14 @@
         <v>-2.5499999999999998</v>
       </c>
       <c r="F17" t="str">
-        <f>IF(G17&lt;0.05,CONCATENATE(ROUND(G17,3),"*"),ROUND(G17,3))</f>
+        <f t="shared" si="0"/>
         <v>0.045*</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>4.48E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>18</v>
       </c>
@@ -9822,14 +9981,14 @@
         <v>-1.01</v>
       </c>
       <c r="F18">
-        <f>IF(G18&lt;0.05,CONCATENATE(ROUND(G18,3),"*"),ROUND(G18,3))</f>
+        <f t="shared" si="0"/>
         <v>0.36199999999999999</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>19</v>
       </c>
@@ -9846,14 +10005,14 @@
         <v>-2.66</v>
       </c>
       <c r="F19" t="str">
-        <f>IF(G19&lt;0.05,CONCATENATE(ROUND(G19,3),"*"),ROUND(G19,3))</f>
+        <f t="shared" si="0"/>
         <v>0.029*</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>20</v>
       </c>
@@ -9870,14 +10029,14 @@
         <v>-1.77</v>
       </c>
       <c r="F20">
-        <f>IF(G20&lt;0.05,CONCATENATE(ROUND(G20,3),"*"),ROUND(G20,3))</f>
+        <f t="shared" si="0"/>
         <v>0.11799999999999999</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>0.1177</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>21</v>
       </c>
@@ -9894,14 +10053,14 @@
         <v>-2.0699999999999998</v>
       </c>
       <c r="F21">
-        <f>IF(G21&lt;0.05,CONCATENATE(ROUND(G21,3),"*"),ROUND(G21,3))</f>
+        <f t="shared" si="0"/>
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>7.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>22</v>
       </c>
@@ -9918,14 +10077,14 @@
         <v>-2.6</v>
       </c>
       <c r="F22" t="str">
-        <f>IF(G22&lt;0.05,CONCATENATE(ROUND(G22,3),"*"),ROUND(G22,3))</f>
+        <f t="shared" si="0"/>
         <v>0.032*</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>23</v>
       </c>
@@ -9942,14 +10101,14 @@
         <v>-2.64</v>
       </c>
       <c r="F23">
-        <f>IF(G23&lt;0.05,CONCATENATE(ROUND(G23,3),"*"),ROUND(G23,3))</f>
+        <f t="shared" si="0"/>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>7.2900000000000006E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>24</v>
       </c>
@@ -9966,14 +10125,14 @@
         <v>-2.96</v>
       </c>
       <c r="F24" t="str">
-        <f>IF(G24&lt;0.05,CONCATENATE(ROUND(G24,3),"*"),ROUND(G24,3))</f>
+        <f t="shared" si="0"/>
         <v>0.036*</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>3.6400000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>25</v>
       </c>
@@ -9990,14 +10149,14 @@
         <v>0.41</v>
       </c>
       <c r="F25">
-        <f>IF(G25&lt;0.05,CONCATENATE(ROUND(G25,3),"*"),ROUND(G25,3))</f>
+        <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>0.71030000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>26</v>
       </c>
@@ -10014,14 +10173,14 @@
         <v>-2.79</v>
       </c>
       <c r="F26" t="str">
-        <f>IF(G26&lt;0.05,CONCATENATE(ROUND(G26,3),"*"),ROUND(G26,3))</f>
+        <f t="shared" si="0"/>
         <v>0.025*</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>2.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>27</v>
       </c>
@@ -10038,43 +10197,16 @@
         <v>-3.13</v>
       </c>
       <c r="F27" t="str">
-        <f>IF(G27&lt;0.05,CONCATENATE(ROUND(G27,3),"*"),ROUND(G27,3))</f>
+        <f t="shared" si="0"/>
         <v>0.016*</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="1:7" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="1:7" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="1:7" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="32" spans="1:7" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="36" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="37" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="39" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="40" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="41" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="42" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="44" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="45" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="46" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10090,7 +10222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFB1076-8356-7A4B-BA71-77A67C3F751C}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+    <sheetView zoomScale="157" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -10102,658 +10234,658 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="14" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>0.93</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f>IF(G4&lt;0.05,CONCATENATE(ROUND(G4,3),"*"),ROUND(G4,3))</f>
         <v>0.35399999999999998</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>0.35370000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="19">
+      <c r="A5" s="18">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="19">
         <v>-1.34</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <f t="shared" ref="F5:F29" si="0">IF(G5&lt;0.05,CONCATENATE(ROUND(G5,3),"*"),ROUND(G5,3))</f>
         <v>0.185</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="20">
         <v>0.18479999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>0.02</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>0.98799999999999999</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <v>0.98760000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>5</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="19">
         <v>1.18</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>0.24299999999999999</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="20">
         <v>0.24299999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>0.35</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>0.72699999999999998</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>0.72719999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <v>7</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <v>1.5</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>0.13900000000000001</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="20">
         <v>0.13880000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>8</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>-0.46</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>0.64500000000000002</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>0.64490000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="19">
+      <c r="A11" s="18">
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <v>0.95</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>0.34899999999999998</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="20">
         <v>0.34920000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>10</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>-0.46</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>0.64400000000000002</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>0.64359999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>11</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="19">
         <v>0.01</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="20">
         <v>0.98980000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>12</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="16">
         <v>-0.36</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <f t="shared" si="0"/>
         <v>0.71899999999999997</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="17">
         <v>0.71919999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>13</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <f t="shared" si="0"/>
         <v>0.57099999999999995</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>0.57089999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>14</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>0.17</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <f t="shared" si="0"/>
         <v>0.86899999999999999</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="17">
         <v>0.86850000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="19">
+      <c r="A17" s="18">
         <v>15</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <v>-1.91</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <f t="shared" si="0"/>
         <v>6.2E-2</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>6.1499999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>16</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <v>2.31</v>
       </c>
-      <c r="F18" s="8" t="str">
+      <c r="F18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0.025*</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="17">
         <v>2.46E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>17</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="19">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F19" s="8" t="str">
+      <c r="F19" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0.016*</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="20">
         <v>1.6400000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>18</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <v>1.91</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <f t="shared" si="0"/>
         <v>6.2E-2</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="17">
         <v>6.1499999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="19">
+      <c r="A21" s="18">
         <v>19</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="19">
         <v>1.96</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <f t="shared" si="0"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="20">
         <v>5.4300000000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <v>20</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="16">
         <v>2.06</v>
       </c>
-      <c r="F22" s="8" t="str">
+      <c r="F22" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0.044*</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="17">
         <v>4.4299999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="19">
+      <c r="A23" s="18">
         <v>21</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="19">
         <v>1.41</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <f t="shared" si="0"/>
         <v>0.16500000000000001</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="20">
         <v>0.1646</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="16">
+      <c r="A24" s="15">
         <v>22</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="16">
         <v>1.04</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="17">
         <v>0.3004</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="19">
+      <c r="A25" s="18">
         <v>23</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="19">
         <v>1.6</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <f t="shared" si="0"/>
         <v>0.11700000000000001</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="20">
         <v>0.11650000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>24</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="16">
         <v>1.66</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <f t="shared" si="0"/>
         <v>0.10199999999999999</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="17">
         <v>0.10199999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="19">
+      <c r="A27" s="18">
         <v>25</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="19">
         <v>-0.27</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <f t="shared" si="0"/>
         <v>0.78500000000000003</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="20">
         <v>0.78510000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="16">
+      <c r="A28" s="15">
         <v>26</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="16">
         <v>2.3199999999999998</v>
       </c>
-      <c r="F28" s="8" t="str">
+      <c r="F28" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0.024*</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="17">
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="9">
+      <c r="A29" s="8">
         <v>27</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>2.2200000000000002</v>
       </c>
-      <c r="F29" s="8" t="str">
+      <c r="F29" s="7" t="str">
         <f t="shared" si="0"/>
         <v>0.031*</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="11">
         <v>3.0700000000000002E-2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>